<commit_message>
update copy for lines with only new timetable PDFs
</commit_message>
<xml_diff>
--- a/src/_data/2023-12/dec-2023-translations.xlsx
+++ b/src/_data/2023-12/dec-2023-translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\nina\LACMTA\mybus-v3\src\_data\2023-12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B92378-B9E2-4FE9-9F03-338AD5672963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A906DA4D-7CA3-4E17-AAC5-682D347FEA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="510" windowWidth="34665" windowHeight="20745" tabRatio="215" firstSheet="1" activeTab="1" xr2:uid="{61E896D0-D03E-8B43-AD1B-B1FBB720644D}"/>
+    <workbookView xWindow="675" yWindow="315" windowWidth="32220" windowHeight="20745" tabRatio="215" firstSheet="1" activeTab="1" xr2:uid="{61E896D0-D03E-8B43-AD1B-B1FBB720644D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2394" uniqueCount="1129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2394" uniqueCount="1131">
   <si>
     <t>English</t>
   </si>
@@ -21612,12 +21612,18 @@
   <si>
     <t>Weekday midday and Saturday/Sunday 9 am to 7 pm trains will operate every 10 minutes instead of 15 minutes.</t>
   </si>
+  <si>
+    <t>Cambios menores en el horario.</t>
+  </si>
+  <si>
+    <t>Minor changes to schedule.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -21793,6 +21799,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -21834,7 +21846,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -21967,6 +21979,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{21294A63-57E9-4EB8-A627-531329A3AEFB}"/>
@@ -23895,10 +23910,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3379E4E-7E82-4114-9EA0-C7AA1E3C9292}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:S89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="15"/>
@@ -23907,7 +23923,8 @@
     <col min="2" max="2" width="14" style="31" customWidth="1"/>
     <col min="3" max="3" width="10.5" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="67" style="31" customWidth="1"/>
-    <col min="5" max="19" width="10.625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="33.75" style="31" customWidth="1"/>
+    <col min="6" max="19" width="10.625" style="31" customWidth="1"/>
     <col min="20" max="16384" width="8.75" style="31"/>
   </cols>
   <sheetData>
@@ -23979,13 +23996,13 @@
       </c>
       <c r="C2" s="42"/>
       <c r="D2" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E2" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G2" s="40" t="s">
         <v>916</v>
@@ -24027,7 +24044,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" hidden="1">
       <c r="A3" s="42">
         <v>4</v>
       </c>
@@ -24095,55 +24112,55 @@
       </c>
       <c r="C4" s="43"/>
       <c r="D4" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>431</v>
+        <v>1130</v>
+      </c>
+      <c r="E4" s="54" t="s">
+        <v>429</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G4" s="40" t="s">
-        <v>916</v>
+        <v>1129</v>
+      </c>
+      <c r="G4" s="42" t="s">
+        <v>558</v>
       </c>
       <c r="H4" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="I4" s="41" t="s">
-        <v>917</v>
+      <c r="I4" s="42" t="s">
+        <v>543</v>
       </c>
       <c r="J4" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="K4" s="41" t="s">
-        <v>529</v>
+      <c r="K4" s="42" t="s">
+        <v>527</v>
       </c>
       <c r="L4" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="M4" s="41" t="s">
-        <v>918</v>
+      <c r="M4" s="42" t="s">
+        <v>512</v>
       </c>
       <c r="N4" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="O4" s="41" t="s">
-        <v>919</v>
+      <c r="O4" s="42" t="s">
+        <v>497</v>
       </c>
       <c r="P4" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="Q4" s="41" t="s">
-        <v>920</v>
+      <c r="Q4" s="42" t="s">
+        <v>482</v>
       </c>
       <c r="R4" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="S4" s="41" t="s">
-        <v>469</v>
+      <c r="S4" s="42" t="s">
+        <v>467</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" hidden="1">
       <c r="A5" s="42">
         <v>14</v>
       </c>
@@ -24200,7 +24217,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" hidden="1">
       <c r="A6" s="42">
         <v>16</v>
       </c>
@@ -24257,7 +24274,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" hidden="1">
       <c r="A7" s="42">
         <v>18</v>
       </c>
@@ -24323,13 +24340,13 @@
       </c>
       <c r="C8" s="43"/>
       <c r="D8" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E8" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G8" s="40" t="s">
         <v>916</v>
@@ -24371,7 +24388,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" hidden="1">
       <c r="A9" s="42">
         <v>28</v>
       </c>
@@ -24428,7 +24445,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" hidden="1">
       <c r="A10" s="42">
         <v>30</v>
       </c>
@@ -24485,7 +24502,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" hidden="1">
       <c r="A11" s="42">
         <v>33</v>
       </c>
@@ -24542,7 +24559,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" hidden="1">
       <c r="A12" s="42">
         <v>35</v>
       </c>
@@ -24608,13 +24625,13 @@
       </c>
       <c r="C13" s="43"/>
       <c r="D13" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E13" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G13" s="40" t="s">
         <v>916</v>
@@ -24656,7 +24673,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" hidden="1">
       <c r="A14" s="42">
         <v>38</v>
       </c>
@@ -24713,7 +24730,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" hidden="1">
       <c r="A15" s="42">
         <v>40</v>
       </c>
@@ -24770,7 +24787,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" hidden="1">
       <c r="A16" s="42">
         <v>45</v>
       </c>
@@ -24827,7 +24844,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" hidden="1">
       <c r="A17" s="42">
         <v>48</v>
       </c>
@@ -24884,7 +24901,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" hidden="1">
       <c r="A18" s="42">
         <v>51</v>
       </c>
@@ -24941,7 +24958,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" hidden="1">
       <c r="A19" s="42">
         <v>53</v>
       </c>
@@ -25000,7 +25017,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" hidden="1">
       <c r="A20" s="42">
         <v>55</v>
       </c>
@@ -25066,52 +25083,52 @@
       </c>
       <c r="C21" s="43"/>
       <c r="D21" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>431</v>
+        <v>1130</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>429</v>
       </c>
       <c r="F21" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G21" s="40" t="s">
-        <v>916</v>
+        <v>1129</v>
+      </c>
+      <c r="G21" s="42" t="s">
+        <v>558</v>
       </c>
       <c r="H21" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="I21" s="41" t="s">
-        <v>917</v>
+      <c r="I21" s="42" t="s">
+        <v>543</v>
       </c>
       <c r="J21" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="K21" s="41" t="s">
-        <v>529</v>
+      <c r="K21" s="42" t="s">
+        <v>527</v>
       </c>
       <c r="L21" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="M21" s="41" t="s">
-        <v>918</v>
+      <c r="M21" s="42" t="s">
+        <v>512</v>
       </c>
       <c r="N21" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="O21" s="41" t="s">
-        <v>919</v>
+      <c r="O21" s="42" t="s">
+        <v>497</v>
       </c>
       <c r="P21" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="Q21" s="41" t="s">
-        <v>920</v>
+      <c r="Q21" s="42" t="s">
+        <v>482</v>
       </c>
       <c r="R21" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="S21" s="41" t="s">
-        <v>469</v>
+      <c r="S21" s="42" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="22" spans="1:19">
@@ -25123,13 +25140,13 @@
       </c>
       <c r="C22" s="43"/>
       <c r="D22" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E22" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F22" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G22" s="40" t="s">
         <v>916</v>
@@ -25171,7 +25188,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" hidden="1">
       <c r="A23" s="42">
         <v>66</v>
       </c>
@@ -25235,52 +25252,52 @@
       </c>
       <c r="C24" s="43"/>
       <c r="D24" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="E24" s="41" t="s">
-        <v>431</v>
+        <v>1130</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>429</v>
       </c>
       <c r="F24" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G24" s="40" t="s">
-        <v>916</v>
+        <v>1129</v>
+      </c>
+      <c r="G24" s="42" t="s">
+        <v>558</v>
       </c>
       <c r="H24" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="I24" s="41" t="s">
-        <v>917</v>
+      <c r="I24" s="42" t="s">
+        <v>543</v>
       </c>
       <c r="J24" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="K24" s="41" t="s">
-        <v>529</v>
+      <c r="K24" s="42" t="s">
+        <v>527</v>
       </c>
       <c r="L24" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="M24" s="41" t="s">
-        <v>918</v>
+      <c r="M24" s="42" t="s">
+        <v>512</v>
       </c>
       <c r="N24" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="O24" s="41" t="s">
-        <v>919</v>
+      <c r="O24" s="42" t="s">
+        <v>497</v>
       </c>
       <c r="P24" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="Q24" s="41" t="s">
-        <v>920</v>
+      <c r="Q24" s="42" t="s">
+        <v>482</v>
       </c>
       <c r="R24" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="S24" s="41" t="s">
-        <v>469</v>
+      <c r="S24" s="42" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="25" spans="1:19">
@@ -25292,13 +25309,13 @@
       </c>
       <c r="C25" s="43"/>
       <c r="D25" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E25" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F25" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G25" s="40" t="s">
         <v>916</v>
@@ -25340,7 +25357,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" hidden="1">
       <c r="A26" s="42">
         <v>90</v>
       </c>
@@ -25408,13 +25425,13 @@
       </c>
       <c r="C27" s="43"/>
       <c r="D27" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E27" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F27" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G27" s="40" t="s">
         <v>916</v>
@@ -25456,7 +25473,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" hidden="1">
       <c r="A28" s="42">
         <v>102</v>
       </c>
@@ -25513,7 +25530,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="32" customFormat="1">
+    <row r="29" spans="1:19" s="32" customFormat="1" hidden="1">
       <c r="A29" s="42">
         <v>105</v>
       </c>
@@ -25570,7 +25587,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" hidden="1">
       <c r="A30" s="42">
         <v>106</v>
       </c>
@@ -25627,7 +25644,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" hidden="1">
       <c r="A31" s="42">
         <v>108</v>
       </c>
@@ -25684,7 +25701,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" hidden="1">
       <c r="A32" s="42">
         <v>110</v>
       </c>
@@ -25741,7 +25758,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" hidden="1">
       <c r="A33" s="42">
         <v>111</v>
       </c>
@@ -25798,7 +25815,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" hidden="1">
       <c r="A34" s="42">
         <v>117</v>
       </c>
@@ -25855,7 +25872,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="35" spans="1:19" s="32" customFormat="1">
+    <row r="35" spans="1:19" s="32" customFormat="1" hidden="1">
       <c r="A35" s="42">
         <v>134</v>
       </c>
@@ -25921,55 +25938,55 @@
       </c>
       <c r="C36" s="43"/>
       <c r="D36" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="E36" s="41" t="s">
-        <v>431</v>
+        <v>1130</v>
+      </c>
+      <c r="E36" s="54" t="s">
+        <v>429</v>
       </c>
       <c r="F36" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G36" s="40" t="s">
-        <v>916</v>
+        <v>1129</v>
+      </c>
+      <c r="G36" s="42" t="s">
+        <v>558</v>
       </c>
       <c r="H36" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="I36" s="41" t="s">
-        <v>917</v>
+      <c r="I36" s="42" t="s">
+        <v>543</v>
       </c>
       <c r="J36" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="K36" s="41" t="s">
-        <v>529</v>
+      <c r="K36" s="42" t="s">
+        <v>527</v>
       </c>
       <c r="L36" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="M36" s="41" t="s">
-        <v>918</v>
+      <c r="M36" s="42" t="s">
+        <v>512</v>
       </c>
       <c r="N36" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="O36" s="41" t="s">
-        <v>919</v>
+      <c r="O36" s="42" t="s">
+        <v>497</v>
       </c>
       <c r="P36" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="Q36" s="41" t="s">
-        <v>920</v>
+      <c r="Q36" s="42" t="s">
+        <v>482</v>
       </c>
       <c r="R36" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="S36" s="41" t="s">
-        <v>469</v>
+      <c r="S36" s="42" t="s">
+        <v>467</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" hidden="1">
       <c r="A37" s="42">
         <v>152</v>
       </c>
@@ -26028,7 +26045,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="38" spans="1:19" s="32" customFormat="1">
+    <row r="38" spans="1:19" s="32" customFormat="1" hidden="1">
       <c r="A38" s="42">
         <v>154</v>
       </c>
@@ -26085,7 +26102,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" hidden="1">
       <c r="A39" s="42">
         <v>155</v>
       </c>
@@ -26142,7 +26159,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" hidden="1">
       <c r="A40" s="42">
         <v>158</v>
       </c>
@@ -26208,13 +26225,13 @@
       </c>
       <c r="C41" s="43"/>
       <c r="D41" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E41" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F41" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G41" s="40" t="s">
         <v>916</v>
@@ -26265,13 +26282,13 @@
       </c>
       <c r="C42" s="43"/>
       <c r="D42" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E42" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F42" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G42" s="40" t="s">
         <v>916</v>
@@ -26322,13 +26339,13 @@
       </c>
       <c r="C43" s="43"/>
       <c r="D43" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E43" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F43" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G43" s="40" t="s">
         <v>916</v>
@@ -26370,7 +26387,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" hidden="1">
       <c r="A44" s="42">
         <v>167</v>
       </c>
@@ -26438,13 +26455,13 @@
       </c>
       <c r="C45" s="43"/>
       <c r="D45" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E45" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F45" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G45" s="40" t="s">
         <v>916</v>
@@ -26495,13 +26512,13 @@
       </c>
       <c r="C46" s="43"/>
       <c r="D46" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E46" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F46" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G46" s="40" t="s">
         <v>916</v>
@@ -26543,7 +26560,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" hidden="1">
       <c r="A47" s="42">
         <v>179</v>
       </c>
@@ -26600,7 +26617,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" hidden="1">
       <c r="A48" s="42">
         <v>180</v>
       </c>
@@ -26659,7 +26676,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" hidden="1">
       <c r="A49" s="42">
         <v>182</v>
       </c>
@@ -26725,55 +26742,55 @@
       </c>
       <c r="C50" s="43"/>
       <c r="D50" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="E50" s="41" t="s">
-        <v>431</v>
+        <v>1130</v>
+      </c>
+      <c r="E50" s="54" t="s">
+        <v>429</v>
       </c>
       <c r="F50" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G50" s="40" t="s">
-        <v>916</v>
+        <v>1129</v>
+      </c>
+      <c r="G50" s="42" t="s">
+        <v>558</v>
       </c>
       <c r="H50" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="I50" s="41" t="s">
-        <v>917</v>
+      <c r="I50" s="42" t="s">
+        <v>543</v>
       </c>
       <c r="J50" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="K50" s="41" t="s">
-        <v>529</v>
+      <c r="K50" s="42" t="s">
+        <v>527</v>
       </c>
       <c r="L50" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="M50" s="41" t="s">
-        <v>918</v>
+      <c r="M50" s="42" t="s">
+        <v>512</v>
       </c>
       <c r="N50" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="O50" s="41" t="s">
-        <v>919</v>
+      <c r="O50" s="42" t="s">
+        <v>497</v>
       </c>
       <c r="P50" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="Q50" s="41" t="s">
-        <v>920</v>
+      <c r="Q50" s="42" t="s">
+        <v>482</v>
       </c>
       <c r="R50" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="S50" s="41" t="s">
-        <v>469</v>
+      <c r="S50" s="42" t="s">
+        <v>467</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" hidden="1">
       <c r="A51" s="42">
         <v>205</v>
       </c>
@@ -26830,7 +26847,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" hidden="1">
       <c r="A52" s="42">
         <v>206</v>
       </c>
@@ -26887,7 +26904,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" hidden="1">
       <c r="A53" s="42">
         <v>207</v>
       </c>
@@ -26944,7 +26961,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="54" spans="1:19">
+    <row r="54" spans="1:19" hidden="1">
       <c r="A54" s="42" t="s">
         <v>1005</v>
       </c>
@@ -27001,7 +27018,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" hidden="1">
       <c r="A55" s="42">
         <v>212</v>
       </c>
@@ -27067,13 +27084,13 @@
       </c>
       <c r="C56" s="43"/>
       <c r="D56" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E56" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F56" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G56" s="40" t="s">
         <v>916</v>
@@ -27115,7 +27132,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" hidden="1">
       <c r="A57" s="42">
         <v>224</v>
       </c>
@@ -27181,13 +27198,13 @@
       </c>
       <c r="C58" s="43"/>
       <c r="D58" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E58" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F58" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G58" s="40" t="s">
         <v>916</v>
@@ -27229,7 +27246,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" hidden="1">
       <c r="A59" s="42">
         <v>232</v>
       </c>
@@ -27286,7 +27303,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" hidden="1">
       <c r="A60" s="42">
         <v>233</v>
       </c>
@@ -27350,13 +27367,13 @@
       </c>
       <c r="C61" s="42"/>
       <c r="D61" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E61" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F61" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G61" s="40" t="s">
         <v>916</v>
@@ -27398,7 +27415,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="62" spans="1:19">
+    <row r="62" spans="1:19" hidden="1">
       <c r="A62" s="42">
         <v>237</v>
       </c>
@@ -27455,7 +27472,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="63" spans="1:19">
+    <row r="63" spans="1:19" hidden="1">
       <c r="A63" s="42">
         <v>240</v>
       </c>
@@ -27512,7 +27529,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="64" spans="1:19">
+    <row r="64" spans="1:19" hidden="1">
       <c r="A64" s="42" t="s">
         <v>1007</v>
       </c>
@@ -27578,13 +27595,13 @@
       </c>
       <c r="C65" s="42"/>
       <c r="D65" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E65" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F65" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G65" s="40" t="s">
         <v>916</v>
@@ -27626,7 +27643,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="66" spans="1:19">
+    <row r="66" spans="1:19" hidden="1">
       <c r="A66" s="42">
         <v>246</v>
       </c>
@@ -27683,7 +27700,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="67" spans="1:19">
+    <row r="67" spans="1:19" hidden="1">
       <c r="A67" s="42">
         <v>251</v>
       </c>
@@ -27749,13 +27766,13 @@
       </c>
       <c r="C68" s="42"/>
       <c r="D68" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E68" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F68" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G68" s="40" t="s">
         <v>916</v>
@@ -27806,55 +27823,55 @@
       </c>
       <c r="C69" s="42"/>
       <c r="D69" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="E69" s="41" t="s">
-        <v>431</v>
+        <v>1130</v>
+      </c>
+      <c r="E69" s="54" t="s">
+        <v>429</v>
       </c>
       <c r="F69" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G69" s="40" t="s">
-        <v>916</v>
+        <v>1129</v>
+      </c>
+      <c r="G69" s="42" t="s">
+        <v>558</v>
       </c>
       <c r="H69" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="I69" s="41" t="s">
-        <v>917</v>
+      <c r="I69" s="42" t="s">
+        <v>543</v>
       </c>
       <c r="J69" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="K69" s="41" t="s">
-        <v>529</v>
+      <c r="K69" s="42" t="s">
+        <v>527</v>
       </c>
       <c r="L69" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="M69" s="41" t="s">
-        <v>918</v>
+      <c r="M69" s="42" t="s">
+        <v>512</v>
       </c>
       <c r="N69" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="O69" s="41" t="s">
-        <v>919</v>
+      <c r="O69" s="42" t="s">
+        <v>497</v>
       </c>
       <c r="P69" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="Q69" s="41" t="s">
-        <v>920</v>
+      <c r="Q69" s="42" t="s">
+        <v>482</v>
       </c>
       <c r="R69" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="S69" s="41" t="s">
-        <v>469</v>
+      <c r="S69" s="42" t="s">
+        <v>467</v>
       </c>
     </row>
-    <row r="70" spans="1:19">
+    <row r="70" spans="1:19" hidden="1">
       <c r="A70" s="42">
         <v>267</v>
       </c>
@@ -27920,13 +27937,13 @@
       </c>
       <c r="C71" s="42"/>
       <c r="D71" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E71" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F71" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G71" s="40" t="s">
         <v>916</v>
@@ -27968,7 +27985,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="72" spans="1:19">
+    <row r="72" spans="1:19" hidden="1">
       <c r="A72" s="42">
         <v>460</v>
       </c>
@@ -28025,7 +28042,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="73" spans="1:19">
+    <row r="73" spans="1:19" hidden="1">
       <c r="A73" s="42" t="s">
         <v>418</v>
       </c>
@@ -28091,13 +28108,13 @@
       </c>
       <c r="C74" s="42"/>
       <c r="D74" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E74" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F74" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G74" s="40" t="s">
         <v>916</v>
@@ -28148,13 +28165,13 @@
       </c>
       <c r="C75" s="42"/>
       <c r="D75" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E75" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F75" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G75" s="40" t="s">
         <v>916</v>
@@ -28196,7 +28213,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="76" spans="1:19">
+    <row r="76" spans="1:19" hidden="1">
       <c r="A76" s="42">
         <v>602</v>
       </c>
@@ -28262,13 +28279,13 @@
       </c>
       <c r="C77" s="42"/>
       <c r="D77" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E77" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F77" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G77" s="40" t="s">
         <v>916</v>
@@ -28310,7 +28327,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="78" spans="1:19">
+    <row r="78" spans="1:19" hidden="1">
       <c r="A78" s="42">
         <v>617</v>
       </c>
@@ -28376,13 +28393,13 @@
       </c>
       <c r="C79" s="42"/>
       <c r="D79" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E79" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F79" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G79" s="40" t="s">
         <v>916</v>
@@ -28433,13 +28450,13 @@
       </c>
       <c r="C80" s="42"/>
       <c r="D80" s="41" t="s">
-        <v>1025</v>
+        <v>1130</v>
       </c>
       <c r="E80" s="41" t="s">
         <v>431</v>
       </c>
       <c r="F80" s="41" t="s">
-        <v>1025</v>
+        <v>1129</v>
       </c>
       <c r="G80" s="40" t="s">
         <v>916</v>
@@ -28490,55 +28507,55 @@
       </c>
       <c r="C81" s="42"/>
       <c r="D81" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="E81" s="41" t="s">
-        <v>431</v>
+        <v>1130</v>
+      </c>
+      <c r="E81" s="54" t="s">
+        <v>429</v>
       </c>
       <c r="F81" s="41" t="s">
-        <v>1025</v>
-      </c>
-      <c r="G81" s="40" t="s">
-        <v>916</v>
+        <v>1129</v>
+      </c>
+      <c r="G81" s="42" t="s">
+        <v>558</v>
       </c>
       <c r="H81" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="I81" s="41" t="s">
-        <v>917</v>
+      <c r="I81" s="42" t="s">
+        <v>543</v>
       </c>
       <c r="J81" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="K81" s="41" t="s">
-        <v>529</v>
+      <c r="K81" s="42" t="s">
+        <v>527</v>
       </c>
       <c r="L81" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="M81" s="41" t="s">
-        <v>918</v>
+      <c r="M81" s="42" t="s">
+        <v>512</v>
       </c>
       <c r="N81" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="O81" s="41" t="s">
-        <v>919</v>
+      <c r="O81" s="42" t="s">
+        <v>497</v>
       </c>
       <c r="P81" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="Q81" s="41" t="s">
-        <v>920</v>
+      <c r="Q81" s="42" t="s">
+        <v>482</v>
       </c>
       <c r="R81" s="41" t="s">
         <v>1025</v>
       </c>
-      <c r="S81" s="41" t="s">
-        <v>469</v>
+      <c r="S81" s="42" t="s">
+        <v>467</v>
       </c>
     </row>
-    <row r="82" spans="1:19">
+    <row r="82" spans="1:19" hidden="1">
       <c r="A82" s="42">
         <v>761</v>
       </c>
@@ -28595,7 +28612,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="83" spans="1:19" s="33" customFormat="1" ht="15.75">
+    <row r="83" spans="1:19" s="33" customFormat="1" ht="15.75" hidden="1">
       <c r="A83" s="42">
         <v>801</v>
       </c>
@@ -28632,7 +28649,7 @@
       </c>
       <c r="S83" s="41"/>
     </row>
-    <row r="84" spans="1:19" s="33" customFormat="1" ht="15.75">
+    <row r="84" spans="1:19" s="33" customFormat="1" ht="15.75" hidden="1">
       <c r="A84" s="42">
         <v>803</v>
       </c>
@@ -28669,7 +28686,7 @@
       </c>
       <c r="S84" s="41"/>
     </row>
-    <row r="85" spans="1:19" s="33" customFormat="1" ht="15.75">
+    <row r="85" spans="1:19" s="33" customFormat="1" ht="15.75" hidden="1">
       <c r="A85" s="42">
         <v>804</v>
       </c>
@@ -28707,7 +28724,7 @@
       </c>
       <c r="S85" s="41"/>
     </row>
-    <row r="86" spans="1:19" s="33" customFormat="1" ht="18">
+    <row r="86" spans="1:19" s="33" customFormat="1" ht="18" hidden="1">
       <c r="A86" s="42">
         <v>807</v>
       </c>
@@ -28744,7 +28761,7 @@
       </c>
       <c r="S86" s="41"/>
     </row>
-    <row r="87" spans="1:19">
+    <row r="87" spans="1:19" hidden="1">
       <c r="A87" s="42">
         <v>857</v>
       </c>
@@ -28801,7 +28818,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="88" spans="1:19">
+    <row r="88" spans="1:19" s="33" customFormat="1" hidden="1">
       <c r="A88" s="42">
         <v>910</v>
       </c>
@@ -28877,7 +28894,13 @@
       <c r="S89" s="41"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S88" xr:uid="{B3379E4E-7E82-4114-9EA0-C7AA1E3C9292}"/>
+  <autoFilter ref="A1:S88" xr:uid="{B3379E4E-7E82-4114-9EA0-C7AA1E3C9292}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Minor timing changes, please check schedule."/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -30135,8 +30158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A2E5A54-8A5E-4D9F-908C-33D2CB64AF15}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:I22"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>